<commit_message>
none to 90,extreme to 99
</commit_message>
<xml_diff>
--- a/不加剪枝 - 副本.xlsx
+++ b/不加剪枝 - 副本.xlsx
@@ -588,10 +588,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="C97" t="n">
-        <v>7.431999683380127</v>
+        <v>529.2619502544403</v>
       </c>
     </row>
     <row r="98">
@@ -599,10 +599,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="C98" t="n">
-        <v>7.159640789031982</v>
+        <v>563.6283569335938</v>
       </c>
     </row>
     <row r="99">
@@ -610,10 +610,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="C99" t="n">
-        <v>12.5074474811554</v>
+        <v>1635.281559705734</v>
       </c>
     </row>
     <row r="100">
@@ -621,10 +621,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="C100" t="n">
-        <v>9.37457799911499</v>
+        <v>1070.729019641876</v>
       </c>
     </row>
     <row r="101">

</xml_diff>